<commit_message>
output 1 to 4
</commit_message>
<xml_diff>
--- a/EEPA_content.xlsx
+++ b/EEPA_content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egos\Mon Drive\ORDI\PYTHON3\JV\WB7 EAPP tool\EEPA-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588F0667-F879-4EB5-B2E7-04B271A1CD38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3112EB68-A610-44D3-BAE3-6474B8AC5FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="18996" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33804" yWindow="0" windowWidth="27732" windowHeight="16656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pillars" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="354">
   <si>
     <t>idx</t>
   </si>
@@ -1042,6 +1042,75 @@
   </si>
   <si>
     <t>d. Assets are managed at relevant line ministry level</t>
+  </si>
+  <si>
+    <t>Has government assessed its exposure to natural hazards (e.g., earthquake, storm, flood etc.)?</t>
+  </si>
+  <si>
+    <t>a. What type of assessment was undertaken (e.g. informal assessment or specialist assessment models such as probabilistic models)</t>
+  </si>
+  <si>
+    <t>b. If a specialist model (such as a probabilistic catastrophe model) was used, what assets (public, private etc.) and hazards were covered?</t>
+  </si>
+  <si>
+    <t>c. Other comments:</t>
+  </si>
+  <si>
+    <t>Are there any databases or registers which list or record the loss and damage to public assets caused by natural disasters?</t>
+  </si>
+  <si>
+    <t>a. What information does it capture? (Please select all that apply)</t>
+  </si>
+  <si>
+    <t>i. Public asset repair costs due to catastrophic events above a certain threshold</t>
+  </si>
+  <si>
+    <t>ii. Public asset repair costs from all types of loss events including smaller loss events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iii. The costs of public asset service interruption (e.g., duration of closure and costs associated with managing disruption) </t>
+  </si>
+  <si>
+    <t>iv. Other:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the government quantified the costs that it could incur from future natural disasters (i.e., the government’s contingent liabilities)?  </t>
+  </si>
+  <si>
+    <t>If yes, please select all that apply:</t>
+  </si>
+  <si>
+    <t>a. The methodology to quantify the contingent liabilities is documented and can be replicated.</t>
+  </si>
+  <si>
+    <t>b. The government accounts for the disaster related contingent liabilities from public assets in any fiscal forecasts, stress test or sensitivity analysis.</t>
+  </si>
+  <si>
+    <t>c. The government publishes a fiscal risk statement that integrates disaster related contingent liabilities from public assets into broader fiscal planning.</t>
+  </si>
+  <si>
+    <t>d. The government accounts for explicit government guarantees for asset damages incurred to public assets owned by subnational government, state owned-enterprises (SOEs) and/or operated through public-private partnerships (PPPs).</t>
+  </si>
+  <si>
+    <t>e. Other:</t>
+  </si>
+  <si>
+    <t>Does the government have risk management policies and/or measures in place to protect public assets prior to natural disasters occurring?</t>
+  </si>
+  <si>
+    <t>Please select all that apply:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. The government has a plan or policy for making public assets more resilient against disaster and climate risks. </t>
+  </si>
+  <si>
+    <t>b. The government has budget allocation processes in place to cover ongoing disaster risk management costs, and climate change adaptation spending for public assets.</t>
+  </si>
+  <si>
+    <t>c. The government has a risk reduction investment plan for its public assets.</t>
+  </si>
+  <si>
+    <t>d. The government has a system or process to track investments which reduce risks to public assets and make them more resilient.</t>
   </si>
 </sst>
 </file>
@@ -1522,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1918,6 +1987,405 @@
       </c>
       <c r="E23" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>6</v>
+      </c>
+      <c r="B24" s="7">
+        <v>2</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>6</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>6</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>6</v>
+      </c>
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7">
+        <v>2</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>7</v>
+      </c>
+      <c r="B28" s="7">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>7</v>
+      </c>
+      <c r="B29" s="7">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>7</v>
+      </c>
+      <c r="B30" s="7">
+        <v>2</v>
+      </c>
+      <c r="C30" s="7">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>7</v>
+      </c>
+      <c r="B31" s="7">
+        <v>2</v>
+      </c>
+      <c r="C31" s="7">
+        <v>2</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>7</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2</v>
+      </c>
+      <c r="C32" s="7">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>7</v>
+      </c>
+      <c r="B33" s="7">
+        <v>2</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>8</v>
+      </c>
+      <c r="B34" s="7">
+        <v>2</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>8</v>
+      </c>
+      <c r="B35" s="7">
+        <v>2</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>8</v>
+      </c>
+      <c r="B36" s="7">
+        <v>2</v>
+      </c>
+      <c r="C36" s="7">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>8</v>
+      </c>
+      <c r="B37" s="7">
+        <v>2</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>8</v>
+      </c>
+      <c r="B38" s="7">
+        <v>2</v>
+      </c>
+      <c r="C38" s="7">
+        <v>2</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>8</v>
+      </c>
+      <c r="B39" s="7">
+        <v>2</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>8</v>
+      </c>
+      <c r="B40" s="7">
+        <v>2</v>
+      </c>
+      <c r="C40" s="7">
+        <v>2</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>9</v>
+      </c>
+      <c r="B41" s="7">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>9</v>
+      </c>
+      <c r="B42" s="7">
+        <v>3</v>
+      </c>
+      <c r="C42" s="7">
+        <v>2</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>9</v>
+      </c>
+      <c r="B43" s="7">
+        <v>3</v>
+      </c>
+      <c r="C43" s="7">
+        <v>2</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>9</v>
+      </c>
+      <c r="B44" s="7">
+        <v>3</v>
+      </c>
+      <c r="C44" s="7">
+        <v>2</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7">
+        <v>9</v>
+      </c>
+      <c r="B45" s="7">
+        <v>3</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>9</v>
+      </c>
+      <c r="B46" s="7">
+        <v>3</v>
+      </c>
+      <c r="C46" s="7">
+        <v>2</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
+        <v>9</v>
+      </c>
+      <c r="B47" s="7">
+        <v>3</v>
+      </c>
+      <c r="C47" s="7">
+        <v>2</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>